<commit_message>
Force Python 3.10 for Streamlit compatibility
</commit_message>
<xml_diff>
--- a/all_vids_info.xlsx
+++ b/all_vids_info.xlsx
@@ -517,10 +517,10 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>624</v>
+        <v>1005</v>
       </c>
       <c r="G2" t="n">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -528,7 +528,7 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -566,10 +566,10 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>8718</v>
+        <v>8987</v>
       </c>
       <c r="G3" t="n">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -577,7 +577,7 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -615,10 +615,10 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>15380</v>
+        <v>15543</v>
       </c>
       <c r="G4" t="n">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -664,10 +664,10 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>8468</v>
+        <v>8546</v>
       </c>
       <c r="G5" t="n">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -713,10 +713,10 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>34169</v>
+        <v>34447</v>
       </c>
       <c r="G6" t="n">
-        <v>684</v>
+        <v>690</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -762,10 +762,10 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>21481</v>
+        <v>21666</v>
       </c>
       <c r="G7" t="n">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -811,10 +811,10 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>13708</v>
+        <v>13746</v>
       </c>
       <c r="G8" t="n">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -860,10 +860,10 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>16242</v>
+        <v>16292</v>
       </c>
       <c r="G9" t="n">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -909,10 +909,10 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>24194</v>
+        <v>24302</v>
       </c>
       <c r="G10" t="n">
-        <v>1673</v>
+        <v>1676</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -958,7 +958,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>16003</v>
+        <v>16041</v>
       </c>
       <c r="G11" t="n">
         <v>833</v>
@@ -1007,10 +1007,10 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>104521</v>
+        <v>104554</v>
       </c>
       <c r="G12" t="n">
-        <v>3573</v>
+        <v>3574</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1056,7 +1056,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>17476</v>
+        <v>17479</v>
       </c>
       <c r="G13" t="n">
         <v>847</v>
@@ -1154,7 +1154,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>15492</v>
+        <v>15542</v>
       </c>
       <c r="G15" t="n">
         <v>787</v>
@@ -1203,10 +1203,10 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>15074</v>
+        <v>15099</v>
       </c>
       <c r="G16" t="n">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1252,10 +1252,10 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>13842</v>
+        <v>13874</v>
       </c>
       <c r="G17" t="n">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1350,10 +1350,10 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>12069</v>
+        <v>12094</v>
       </c>
       <c r="G19" t="n">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1399,10 +1399,10 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1544981</v>
+        <v>1547447</v>
       </c>
       <c r="G20" t="n">
-        <v>32446</v>
+        <v>32487</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1448,7 +1448,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>62612</v>
+        <v>62613</v>
       </c>
       <c r="G21" t="n">
         <v>3278</v>
@@ -1546,10 +1546,10 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>23794</v>
+        <v>23817</v>
       </c>
       <c r="G23" t="n">
-        <v>1424</v>
+        <v>1426</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1595,7 +1595,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>32577</v>
+        <v>32580</v>
       </c>
       <c r="G24" t="n">
         <v>1630</v>
@@ -1606,7 +1606,7 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>4344</v>
+        <v>4345</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1644,7 +1644,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>39001</v>
+        <v>39021</v>
       </c>
       <c r="G25" t="n">
         <v>2354</v>
@@ -1742,10 +1742,10 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>17670</v>
+        <v>17687</v>
       </c>
       <c r="G27" t="n">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1791,7 +1791,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>16685</v>
+        <v>16698</v>
       </c>
       <c r="G28" t="n">
         <v>1012</v>
@@ -1840,10 +1840,10 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>55235</v>
+        <v>55259</v>
       </c>
       <c r="G29" t="n">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -1889,10 +1889,10 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>230896</v>
+        <v>230912</v>
       </c>
       <c r="G30" t="n">
-        <v>6404</v>
+        <v>6405</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -1900,7 +1900,7 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -1938,10 +1938,10 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>75609</v>
+        <v>75665</v>
       </c>
       <c r="G31" t="n">
-        <v>4157</v>
+        <v>4160</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -1990,7 +1990,7 @@
         <v>103937</v>
       </c>
       <c r="G32" t="n">
-        <v>2881</v>
+        <v>2880</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -2085,10 +2085,10 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>86146</v>
+        <v>86272</v>
       </c>
       <c r="G34" t="n">
-        <v>5025</v>
+        <v>5033</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
@@ -2134,10 +2134,10 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>433223</v>
+        <v>433275</v>
       </c>
       <c r="G35" t="n">
-        <v>12973</v>
+        <v>12975</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -2183,7 +2183,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>14778</v>
+        <v>14784</v>
       </c>
       <c r="G36" t="n">
         <v>848</v>
@@ -2281,10 +2281,10 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>19735</v>
+        <v>19746</v>
       </c>
       <c r="G38" t="n">
-        <v>2104</v>
+        <v>2105</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
@@ -2379,7 +2379,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>12840</v>
+        <v>12843</v>
       </c>
       <c r="G40" t="n">
         <v>1097</v>
@@ -2428,7 +2428,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>9167</v>
+        <v>9170</v>
       </c>
       <c r="G41" t="n">
         <v>591</v>
@@ -2526,7 +2526,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>72441</v>
+        <v>72478</v>
       </c>
       <c r="G43" t="n">
         <v>2021</v>
@@ -2575,7 +2575,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>9404</v>
+        <v>9409</v>
       </c>
       <c r="G44" t="n">
         <v>841</v>
@@ -2771,10 +2771,10 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>98339</v>
+        <v>98361</v>
       </c>
       <c r="G48" t="n">
-        <v>2573</v>
+        <v>2574</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
@@ -2820,7 +2820,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>13445</v>
+        <v>13448</v>
       </c>
       <c r="G49" t="n">
         <v>1247</v>
@@ -2918,7 +2918,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>12520</v>
+        <v>12524</v>
       </c>
       <c r="G51" t="n">
         <v>945</v>
@@ -3016,7 +3016,7 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>132137</v>
+        <v>132164</v>
       </c>
       <c r="G53" t="n">
         <v>2954</v>
@@ -3065,7 +3065,7 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>13206</v>
+        <v>13209</v>
       </c>
       <c r="G54" t="n">
         <v>1327</v>
@@ -3114,7 +3114,7 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>31944</v>
+        <v>31945</v>
       </c>
       <c r="G55" t="n">
         <v>1029</v>
@@ -3163,7 +3163,7 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>13503</v>
+        <v>13505</v>
       </c>
       <c r="G56" t="n">
         <v>1105</v>
@@ -3261,10 +3261,10 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>156923</v>
+        <v>156983</v>
       </c>
       <c r="G58" t="n">
-        <v>3691</v>
+        <v>3692</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
@@ -3310,7 +3310,7 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>104433</v>
+        <v>104467</v>
       </c>
       <c r="G59" t="n">
         <v>2436</v>
@@ -3359,7 +3359,7 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>196812</v>
+        <v>196868</v>
       </c>
       <c r="G60" t="n">
         <v>4802</v>
@@ -3604,7 +3604,7 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>143101</v>
+        <v>143113</v>
       </c>
       <c r="G65" t="n">
         <v>3351</v>
@@ -3653,7 +3653,7 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>12268</v>
+        <v>12269</v>
       </c>
       <c r="G66" t="n">
         <v>910</v>
@@ -3702,10 +3702,10 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>91416</v>
+        <v>91435</v>
       </c>
       <c r="G67" t="n">
-        <v>2752</v>
+        <v>2753</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
@@ -3751,10 +3751,10 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>332561</v>
+        <v>332986</v>
       </c>
       <c r="G68" t="n">
-        <v>22076</v>
+        <v>22090</v>
       </c>
       <c r="H68" t="inlineStr">
         <is>
@@ -3849,7 +3849,7 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>244016</v>
+        <v>244065</v>
       </c>
       <c r="G70" t="n">
         <v>5057</v>
@@ -3947,10 +3947,10 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>19505</v>
+        <v>19507</v>
       </c>
       <c r="G72" t="n">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
@@ -3996,7 +3996,7 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>195567</v>
+        <v>195628</v>
       </c>
       <c r="G73" t="n">
         <v>4378</v>
@@ -4045,10 +4045,10 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>8736</v>
+        <v>8737</v>
       </c>
       <c r="G74" t="n">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
@@ -4143,10 +4143,10 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>11476</v>
+        <v>11478</v>
       </c>
       <c r="G76" t="n">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
@@ -4192,7 +4192,7 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>11119</v>
+        <v>11121</v>
       </c>
       <c r="G77" t="n">
         <v>1240</v>
@@ -4241,10 +4241,10 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>114456</v>
+        <v>114471</v>
       </c>
       <c r="G78" t="n">
-        <v>2638</v>
+        <v>2639</v>
       </c>
       <c r="H78" t="inlineStr">
         <is>
@@ -4290,10 +4290,10 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>138477</v>
+        <v>138527</v>
       </c>
       <c r="G79" t="n">
-        <v>3343</v>
+        <v>3344</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
@@ -4339,7 +4339,7 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>10310</v>
+        <v>10313</v>
       </c>
       <c r="G80" t="n">
         <v>918</v>
@@ -4388,7 +4388,7 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>13433</v>
+        <v>13434</v>
       </c>
       <c r="G81" t="n">
         <v>1304</v>
@@ -4437,10 +4437,10 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>136692</v>
+        <v>136739</v>
       </c>
       <c r="G82" t="n">
-        <v>3346</v>
+        <v>3344</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
@@ -4486,7 +4486,7 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>74602</v>
+        <v>74612</v>
       </c>
       <c r="G83" t="n">
         <v>2253</v>
@@ -4633,10 +4633,10 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>295474</v>
+        <v>295527</v>
       </c>
       <c r="G86" t="n">
-        <v>6049</v>
+        <v>6052</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
@@ -4829,7 +4829,7 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>45664</v>
+        <v>45667</v>
       </c>
       <c r="G90" t="n">
         <v>2143</v>
@@ -4976,7 +4976,7 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>32530</v>
+        <v>32532</v>
       </c>
       <c r="G93" t="n">
         <v>1414</v>
@@ -5074,10 +5074,10 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>180028</v>
+        <v>180127</v>
       </c>
       <c r="G95" t="n">
-        <v>4210</v>
+        <v>4212</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
@@ -5123,10 +5123,10 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>11705</v>
+        <v>11706</v>
       </c>
       <c r="G96" t="n">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
@@ -5172,10 +5172,10 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>67364</v>
+        <v>67391</v>
       </c>
       <c r="G97" t="n">
-        <v>2074</v>
+        <v>2075</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
@@ -5368,7 +5368,7 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>13837</v>
+        <v>13838</v>
       </c>
       <c r="G101" t="n">
         <v>1648</v>
@@ -5417,7 +5417,7 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>38733</v>
+        <v>38740</v>
       </c>
       <c r="G102" t="n">
         <v>1153</v>
@@ -5466,7 +5466,7 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>42641</v>
+        <v>42660</v>
       </c>
       <c r="G103" t="n">
         <v>2322</v>
@@ -5613,7 +5613,7 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>32780</v>
+        <v>32784</v>
       </c>
       <c r="G106" t="n">
         <v>3357</v>
@@ -5662,10 +5662,10 @@
         </is>
       </c>
       <c r="F107" t="n">
-        <v>39787</v>
+        <v>39834</v>
       </c>
       <c r="G107" t="n">
-        <v>1319</v>
+        <v>1320</v>
       </c>
       <c r="H107" t="inlineStr">
         <is>
@@ -5673,7 +5673,7 @@
         </is>
       </c>
       <c r="I107" t="n">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="J107" t="inlineStr">
         <is>
@@ -5858,7 +5858,7 @@
         </is>
       </c>
       <c r="F111" t="n">
-        <v>41728</v>
+        <v>41785</v>
       </c>
       <c r="G111" t="n">
         <v>1283</v>
@@ -5869,7 +5869,7 @@
         </is>
       </c>
       <c r="I111" t="n">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="J111" t="inlineStr">
         <is>
@@ -5907,7 +5907,7 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>17646</v>
+        <v>17647</v>
       </c>
       <c r="G112" t="n">
         <v>1208</v>
@@ -5956,7 +5956,7 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>47837</v>
+        <v>47918</v>
       </c>
       <c r="G113" t="n">
         <v>1508</v>
@@ -6005,7 +6005,7 @@
         </is>
       </c>
       <c r="F114" t="n">
-        <v>8903</v>
+        <v>8904</v>
       </c>
       <c r="G114" t="n">
         <v>769</v>
@@ -6054,10 +6054,10 @@
         </is>
       </c>
       <c r="F115" t="n">
-        <v>137196</v>
+        <v>137248</v>
       </c>
       <c r="G115" t="n">
-        <v>3055</v>
+        <v>3057</v>
       </c>
       <c r="H115" t="inlineStr">
         <is>
@@ -6201,10 +6201,10 @@
         </is>
       </c>
       <c r="F118" t="n">
-        <v>67975</v>
+        <v>68003</v>
       </c>
       <c r="G118" t="n">
-        <v>2163</v>
+        <v>2164</v>
       </c>
       <c r="H118" t="inlineStr">
         <is>
@@ -6250,7 +6250,7 @@
         </is>
       </c>
       <c r="F119" t="n">
-        <v>14593</v>
+        <v>14594</v>
       </c>
       <c r="G119" t="n">
         <v>1062</v>
@@ -6397,10 +6397,10 @@
         </is>
       </c>
       <c r="F122" t="n">
-        <v>192217</v>
+        <v>192226</v>
       </c>
       <c r="G122" t="n">
-        <v>4183</v>
+        <v>4184</v>
       </c>
       <c r="H122" t="inlineStr">
         <is>
@@ -6446,10 +6446,10 @@
         </is>
       </c>
       <c r="F123" t="n">
-        <v>158068</v>
+        <v>158182</v>
       </c>
       <c r="G123" t="n">
-        <v>3416</v>
+        <v>3417</v>
       </c>
       <c r="H123" t="inlineStr">
         <is>
@@ -6457,7 +6457,7 @@
         </is>
       </c>
       <c r="I123" t="n">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="J123" t="inlineStr">
         <is>
@@ -6544,10 +6544,10 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>104106</v>
+        <v>104149</v>
       </c>
       <c r="G125" t="n">
-        <v>2365</v>
+        <v>2366</v>
       </c>
       <c r="H125" t="inlineStr">
         <is>
@@ -6593,10 +6593,10 @@
         </is>
       </c>
       <c r="F126" t="n">
-        <v>252305</v>
+        <v>252540</v>
       </c>
       <c r="G126" t="n">
-        <v>5750</v>
+        <v>5756</v>
       </c>
       <c r="H126" t="inlineStr">
         <is>
@@ -6604,7 +6604,7 @@
         </is>
       </c>
       <c r="I126" t="n">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="J126" t="inlineStr">
         <is>
@@ -6642,10 +6642,10 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>268921</v>
+        <v>269103</v>
       </c>
       <c r="G127" t="n">
-        <v>6042</v>
+        <v>6045</v>
       </c>
       <c r="H127" t="inlineStr">
         <is>
@@ -6653,7 +6653,7 @@
         </is>
       </c>
       <c r="I127" t="n">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="J127" t="inlineStr">
         <is>
@@ -6691,7 +6691,7 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>30322</v>
+        <v>30328</v>
       </c>
       <c r="G128" t="n">
         <v>1420</v>
@@ -7083,10 +7083,10 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>504944</v>
+        <v>504988</v>
       </c>
       <c r="G136" t="n">
-        <v>10248</v>
+        <v>10249</v>
       </c>
       <c r="H136" t="inlineStr">
         <is>
@@ -7181,7 +7181,7 @@
         </is>
       </c>
       <c r="F138" t="n">
-        <v>9523</v>
+        <v>9525</v>
       </c>
       <c r="G138" t="n">
         <v>647</v>
@@ -7230,10 +7230,10 @@
         </is>
       </c>
       <c r="F139" t="n">
-        <v>22803</v>
+        <v>22807</v>
       </c>
       <c r="G139" t="n">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="H139" t="inlineStr">
         <is>
@@ -7328,7 +7328,7 @@
         </is>
       </c>
       <c r="F141" t="n">
-        <v>9537</v>
+        <v>9538</v>
       </c>
       <c r="G141" t="n">
         <v>694</v>
@@ -7475,7 +7475,7 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>9005</v>
+        <v>9006</v>
       </c>
       <c r="G144" t="n">
         <v>955</v>
@@ -7723,7 +7723,7 @@
         <v>6789</v>
       </c>
       <c r="G149" t="n">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="H149" t="inlineStr">
         <is>
@@ -7916,7 +7916,7 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>14331</v>
+        <v>14332</v>
       </c>
       <c r="G153" t="n">
         <v>903</v>
@@ -8014,7 +8014,7 @@
         </is>
       </c>
       <c r="F155" t="n">
-        <v>9812</v>
+        <v>9813</v>
       </c>
       <c r="G155" t="n">
         <v>769</v>
@@ -8112,10 +8112,10 @@
         </is>
       </c>
       <c r="F157" t="n">
-        <v>41204</v>
+        <v>41233</v>
       </c>
       <c r="G157" t="n">
-        <v>3208</v>
+        <v>3209</v>
       </c>
       <c r="H157" t="inlineStr">
         <is>
@@ -8406,7 +8406,7 @@
         </is>
       </c>
       <c r="F163" t="n">
-        <v>133025</v>
+        <v>133084</v>
       </c>
       <c r="G163" t="n">
         <v>2896</v>
@@ -8651,10 +8651,10 @@
         </is>
       </c>
       <c r="F168" t="n">
-        <v>676966</v>
+        <v>677039</v>
       </c>
       <c r="G168" t="n">
-        <v>11107</v>
+        <v>11108</v>
       </c>
       <c r="H168" t="inlineStr">
         <is>
@@ -8798,7 +8798,7 @@
         </is>
       </c>
       <c r="F171" t="n">
-        <v>9790</v>
+        <v>9791</v>
       </c>
       <c r="G171" t="n">
         <v>910</v>
@@ -8896,7 +8896,7 @@
         </is>
       </c>
       <c r="F173" t="n">
-        <v>42128</v>
+        <v>42129</v>
       </c>
       <c r="G173" t="n">
         <v>861</v>
@@ -9239,7 +9239,7 @@
         </is>
       </c>
       <c r="F180" t="n">
-        <v>441258</v>
+        <v>441301</v>
       </c>
       <c r="G180" t="n">
         <v>7610</v>
@@ -9386,7 +9386,7 @@
         </is>
       </c>
       <c r="F183" t="n">
-        <v>97822</v>
+        <v>97823</v>
       </c>
       <c r="G183" t="n">
         <v>1891</v>
@@ -9582,7 +9582,7 @@
         </is>
       </c>
       <c r="F187" t="n">
-        <v>23067</v>
+        <v>23074</v>
       </c>
       <c r="G187" t="n">
         <v>2098</v>
@@ -9974,7 +9974,7 @@
         </is>
       </c>
       <c r="F195" t="n">
-        <v>11913</v>
+        <v>11914</v>
       </c>
       <c r="G195" t="n">
         <v>1035</v>
@@ -10072,7 +10072,7 @@
         </is>
       </c>
       <c r="F197" t="n">
-        <v>10426</v>
+        <v>10427</v>
       </c>
       <c r="G197" t="n">
         <v>924</v>
@@ -10121,10 +10121,10 @@
         </is>
       </c>
       <c r="F198" t="n">
-        <v>207284</v>
+        <v>207332</v>
       </c>
       <c r="G198" t="n">
-        <v>4215</v>
+        <v>4216</v>
       </c>
       <c r="H198" t="inlineStr">
         <is>
@@ -10415,7 +10415,7 @@
         </is>
       </c>
       <c r="F204" t="n">
-        <v>15705</v>
+        <v>15706</v>
       </c>
       <c r="G204" t="n">
         <v>1897</v>
@@ -10562,7 +10562,7 @@
         </is>
       </c>
       <c r="F207" t="n">
-        <v>11255</v>
+        <v>11257</v>
       </c>
       <c r="G207" t="n">
         <v>986</v>
@@ -10965,7 +10965,7 @@
         </is>
       </c>
       <c r="I215" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J215" t="inlineStr">
         <is>
@@ -11150,7 +11150,7 @@
         </is>
       </c>
       <c r="F219" t="n">
-        <v>352312</v>
+        <v>352356</v>
       </c>
       <c r="G219" t="n">
         <v>6558</v>
@@ -11199,10 +11199,10 @@
         </is>
       </c>
       <c r="F220" t="n">
-        <v>23035</v>
+        <v>23036</v>
       </c>
       <c r="G220" t="n">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="H220" t="inlineStr">
         <is>
@@ -11346,7 +11346,7 @@
         </is>
       </c>
       <c r="F223" t="n">
-        <v>13541</v>
+        <v>13542</v>
       </c>
       <c r="G223" t="n">
         <v>1827</v>
@@ -11444,7 +11444,7 @@
         </is>
       </c>
       <c r="F225" t="n">
-        <v>12374</v>
+        <v>12375</v>
       </c>
       <c r="G225" t="n">
         <v>1045</v>
@@ -11493,10 +11493,10 @@
         </is>
       </c>
       <c r="F226" t="n">
-        <v>330501</v>
+        <v>330583</v>
       </c>
       <c r="G226" t="n">
-        <v>5623</v>
+        <v>5622</v>
       </c>
       <c r="H226" t="inlineStr">
         <is>
@@ -11542,7 +11542,7 @@
         </is>
       </c>
       <c r="F227" t="n">
-        <v>334124</v>
+        <v>334194</v>
       </c>
       <c r="G227" t="n">
         <v>6180</v>
@@ -11594,7 +11594,7 @@
         <v>13072</v>
       </c>
       <c r="G228" t="n">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="H228" t="inlineStr">
         <is>
@@ -11689,10 +11689,10 @@
         </is>
       </c>
       <c r="F230" t="n">
-        <v>234712</v>
+        <v>234821</v>
       </c>
       <c r="G230" t="n">
-        <v>3772</v>
+        <v>3773</v>
       </c>
       <c r="H230" t="inlineStr">
         <is>
@@ -11700,7 +11700,7 @@
         </is>
       </c>
       <c r="I230" t="n">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="J230" t="inlineStr">
         <is>
@@ -11738,10 +11738,10 @@
         </is>
       </c>
       <c r="F231" t="n">
-        <v>37051</v>
+        <v>37056</v>
       </c>
       <c r="G231" t="n">
-        <v>2257</v>
+        <v>2256</v>
       </c>
       <c r="H231" t="inlineStr">
         <is>
@@ -11787,10 +11787,10 @@
         </is>
       </c>
       <c r="F232" t="n">
-        <v>1279028</v>
+        <v>1279459</v>
       </c>
       <c r="G232" t="n">
-        <v>53878</v>
+        <v>53883</v>
       </c>
       <c r="H232" t="inlineStr">
         <is>
@@ -11836,7 +11836,7 @@
         </is>
       </c>
       <c r="F233" t="n">
-        <v>11280</v>
+        <v>11282</v>
       </c>
       <c r="G233" t="n">
         <v>258</v>
@@ -11937,7 +11937,7 @@
         <v>20504</v>
       </c>
       <c r="G235" t="n">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="H235" t="inlineStr">
         <is>
@@ -11983,10 +11983,10 @@
         </is>
       </c>
       <c r="F236" t="n">
-        <v>331784</v>
+        <v>331845</v>
       </c>
       <c r="G236" t="n">
-        <v>5596</v>
+        <v>5600</v>
       </c>
       <c r="H236" t="inlineStr">
         <is>
@@ -12032,10 +12032,10 @@
         </is>
       </c>
       <c r="F237" t="n">
-        <v>501007</v>
+        <v>501028</v>
       </c>
       <c r="G237" t="n">
-        <v>7674</v>
+        <v>7672</v>
       </c>
       <c r="H237" t="inlineStr">
         <is>
@@ -12043,7 +12043,7 @@
         </is>
       </c>
       <c r="I237" t="n">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="J237" t="inlineStr">
         <is>
@@ -12084,7 +12084,7 @@
         <v>18850</v>
       </c>
       <c r="G238" t="n">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="H238" t="inlineStr">
         <is>
@@ -12182,7 +12182,7 @@
         <v>8965</v>
       </c>
       <c r="G240" t="n">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="H240" t="inlineStr">
         <is>
@@ -12228,7 +12228,7 @@
         </is>
       </c>
       <c r="F241" t="n">
-        <v>91026</v>
+        <v>91078</v>
       </c>
       <c r="G241" t="n">
         <v>2032</v>
@@ -12239,7 +12239,7 @@
         </is>
       </c>
       <c r="I241" t="n">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="J241" t="inlineStr">
         <is>
@@ -12277,10 +12277,10 @@
         </is>
       </c>
       <c r="F242" t="n">
-        <v>50887</v>
+        <v>50897</v>
       </c>
       <c r="G242" t="n">
-        <v>2522</v>
+        <v>2521</v>
       </c>
       <c r="H242" t="inlineStr">
         <is>
@@ -12378,7 +12378,7 @@
         <v>20669</v>
       </c>
       <c r="G244" t="n">
-        <v>2769</v>
+        <v>2768</v>
       </c>
       <c r="H244" t="inlineStr">
         <is>
@@ -12424,7 +12424,7 @@
         </is>
       </c>
       <c r="F245" t="n">
-        <v>97906</v>
+        <v>97961</v>
       </c>
       <c r="G245" t="n">
         <v>2287</v>
@@ -12476,7 +12476,7 @@
         <v>17916</v>
       </c>
       <c r="G246" t="n">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="H246" t="inlineStr">
         <is>
@@ -12522,10 +12522,10 @@
         </is>
       </c>
       <c r="F247" t="n">
-        <v>23226</v>
+        <v>23227</v>
       </c>
       <c r="G247" t="n">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="H247" t="inlineStr">
         <is>
@@ -12571,7 +12571,7 @@
         </is>
       </c>
       <c r="F248" t="n">
-        <v>15518</v>
+        <v>15530</v>
       </c>
       <c r="G248" t="n">
         <v>363</v>
@@ -12620,7 +12620,7 @@
         </is>
       </c>
       <c r="F249" t="n">
-        <v>166548</v>
+        <v>166591</v>
       </c>
       <c r="G249" t="n">
         <v>3665</v>
@@ -12669,10 +12669,10 @@
         </is>
       </c>
       <c r="F250" t="n">
-        <v>200685</v>
+        <v>200760</v>
       </c>
       <c r="G250" t="n">
-        <v>4142</v>
+        <v>4143</v>
       </c>
       <c r="H250" t="inlineStr">
         <is>
@@ -12767,10 +12767,10 @@
         </is>
       </c>
       <c r="F252" t="n">
-        <v>38116</v>
+        <v>38179</v>
       </c>
       <c r="G252" t="n">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="H252" t="inlineStr">
         <is>
@@ -12819,7 +12819,7 @@
         <v>61957</v>
       </c>
       <c r="G253" t="n">
-        <v>2825</v>
+        <v>2826</v>
       </c>
       <c r="H253" t="inlineStr">
         <is>
@@ -12865,10 +12865,10 @@
         </is>
       </c>
       <c r="F254" t="n">
-        <v>324366</v>
+        <v>324633</v>
       </c>
       <c r="G254" t="n">
-        <v>6564</v>
+        <v>6566</v>
       </c>
       <c r="H254" t="inlineStr">
         <is>
@@ -12876,7 +12876,7 @@
         </is>
       </c>
       <c r="I254" t="n">
-        <v>1437</v>
+        <v>1438</v>
       </c>
       <c r="J254" t="inlineStr">
         <is>
@@ -12914,10 +12914,10 @@
         </is>
       </c>
       <c r="F255" t="n">
-        <v>372750</v>
+        <v>372827</v>
       </c>
       <c r="G255" t="n">
-        <v>5997</v>
+        <v>5998</v>
       </c>
       <c r="H255" t="inlineStr">
         <is>
@@ -12963,10 +12963,10 @@
         </is>
       </c>
       <c r="F256" t="n">
-        <v>138488</v>
+        <v>138552</v>
       </c>
       <c r="G256" t="n">
-        <v>3681</v>
+        <v>3684</v>
       </c>
       <c r="H256" t="inlineStr">
         <is>
@@ -13012,7 +13012,7 @@
         </is>
       </c>
       <c r="F257" t="n">
-        <v>111179</v>
+        <v>111185</v>
       </c>
       <c r="G257" t="n">
         <v>2180</v>
@@ -13061,10 +13061,10 @@
         </is>
       </c>
       <c r="F258" t="n">
-        <v>19785</v>
+        <v>19806</v>
       </c>
       <c r="G258" t="n">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="H258" t="inlineStr">
         <is>
@@ -13110,10 +13110,10 @@
         </is>
       </c>
       <c r="F259" t="n">
-        <v>52263</v>
+        <v>52264</v>
       </c>
       <c r="G259" t="n">
-        <v>3119</v>
+        <v>3118</v>
       </c>
       <c r="H259" t="inlineStr">
         <is>
@@ -13159,10 +13159,10 @@
         </is>
       </c>
       <c r="F260" t="n">
-        <v>242898</v>
+        <v>243201</v>
       </c>
       <c r="G260" t="n">
-        <v>5817</v>
+        <v>5822</v>
       </c>
       <c r="H260" t="inlineStr">
         <is>
@@ -13306,10 +13306,10 @@
         </is>
       </c>
       <c r="F263" t="n">
-        <v>526448</v>
+        <v>526459</v>
       </c>
       <c r="G263" t="n">
-        <v>14839</v>
+        <v>14837</v>
       </c>
       <c r="H263" t="inlineStr">
         <is>
@@ -13404,7 +13404,7 @@
         </is>
       </c>
       <c r="F265" t="n">
-        <v>320785</v>
+        <v>320795</v>
       </c>
       <c r="G265" t="n">
         <v>7081</v>
@@ -13453,7 +13453,7 @@
         </is>
       </c>
       <c r="F266" t="n">
-        <v>104691</v>
+        <v>104695</v>
       </c>
       <c r="G266" t="n">
         <v>2009</v>
@@ -13502,10 +13502,10 @@
         </is>
       </c>
       <c r="F267" t="n">
-        <v>44659</v>
+        <v>44660</v>
       </c>
       <c r="G267" t="n">
-        <v>3752</v>
+        <v>3751</v>
       </c>
       <c r="H267" t="inlineStr">
         <is>
@@ -13600,10 +13600,10 @@
         </is>
       </c>
       <c r="F269" t="n">
-        <v>629252</v>
+        <v>629260</v>
       </c>
       <c r="G269" t="n">
-        <v>13890</v>
+        <v>13888</v>
       </c>
       <c r="H269" t="inlineStr">
         <is>
@@ -13747,10 +13747,10 @@
         </is>
       </c>
       <c r="F272" t="n">
-        <v>37134</v>
+        <v>37135</v>
       </c>
       <c r="G272" t="n">
-        <v>3292</v>
+        <v>3291</v>
       </c>
       <c r="H272" t="inlineStr">
         <is>
@@ -13796,10 +13796,10 @@
         </is>
       </c>
       <c r="F273" t="n">
-        <v>437469</v>
+        <v>437988</v>
       </c>
       <c r="G273" t="n">
-        <v>8945</v>
+        <v>8954</v>
       </c>
       <c r="H273" t="inlineStr">
         <is>
@@ -13807,7 +13807,7 @@
         </is>
       </c>
       <c r="I273" t="n">
-        <v>3145</v>
+        <v>3147</v>
       </c>
       <c r="J273" t="inlineStr">
         <is>
@@ -13845,10 +13845,10 @@
         </is>
       </c>
       <c r="F274" t="n">
-        <v>924247</v>
+        <v>925970</v>
       </c>
       <c r="G274" t="n">
-        <v>20660</v>
+        <v>20711</v>
       </c>
       <c r="H274" t="inlineStr">
         <is>
@@ -13856,7 +13856,7 @@
         </is>
       </c>
       <c r="I274" t="n">
-        <v>5197</v>
+        <v>5207</v>
       </c>
       <c r="J274" t="inlineStr">
         <is>
@@ -13894,7 +13894,7 @@
         </is>
       </c>
       <c r="F275" t="n">
-        <v>58078</v>
+        <v>58107</v>
       </c>
       <c r="G275" t="n">
         <v>1260</v>
@@ -13943,10 +13943,10 @@
         </is>
       </c>
       <c r="F276" t="n">
-        <v>329873</v>
+        <v>330164</v>
       </c>
       <c r="G276" t="n">
-        <v>6017</v>
+        <v>6021</v>
       </c>
       <c r="H276" t="inlineStr">
         <is>
@@ -13954,7 +13954,7 @@
         </is>
       </c>
       <c r="I276" t="n">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="J276" t="inlineStr">
         <is>
@@ -13992,10 +13992,10 @@
         </is>
       </c>
       <c r="F277" t="n">
-        <v>53148</v>
+        <v>53150</v>
       </c>
       <c r="G277" t="n">
-        <v>4681</v>
+        <v>4680</v>
       </c>
       <c r="H277" t="inlineStr">
         <is>
@@ -14044,7 +14044,7 @@
         <v>39229</v>
       </c>
       <c r="G278" t="n">
-        <v>3183</v>
+        <v>3182</v>
       </c>
       <c r="H278" t="inlineStr">
         <is>
@@ -14090,10 +14090,10 @@
         </is>
       </c>
       <c r="F279" t="n">
-        <v>40779</v>
+        <v>40786</v>
       </c>
       <c r="G279" t="n">
-        <v>2658</v>
+        <v>2657</v>
       </c>
       <c r="H279" t="inlineStr">
         <is>
@@ -14142,7 +14142,7 @@
         <v>19601</v>
       </c>
       <c r="G280" t="n">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="H280" t="inlineStr">
         <is>
@@ -14338,7 +14338,7 @@
         <v>14970</v>
       </c>
       <c r="G284" t="n">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="H284" t="inlineStr">
         <is>
@@ -14433,10 +14433,10 @@
         </is>
       </c>
       <c r="F286" t="n">
-        <v>136239</v>
+        <v>136244</v>
       </c>
       <c r="G286" t="n">
-        <v>8811</v>
+        <v>8810</v>
       </c>
       <c r="H286" t="inlineStr">
         <is>
@@ -14482,10 +14482,10 @@
         </is>
       </c>
       <c r="F287" t="n">
-        <v>30878</v>
+        <v>30879</v>
       </c>
       <c r="G287" t="n">
-        <v>2786</v>
+        <v>2785</v>
       </c>
       <c r="H287" t="inlineStr">
         <is>
@@ -14580,7 +14580,7 @@
         </is>
       </c>
       <c r="F289" t="n">
-        <v>37396</v>
+        <v>37408</v>
       </c>
       <c r="G289" t="n">
         <v>1638</v>
@@ -14632,7 +14632,7 @@
         <v>15551</v>
       </c>
       <c r="G290" t="n">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="H290" t="inlineStr">
         <is>
@@ -14730,7 +14730,7 @@
         <v>10332</v>
       </c>
       <c r="G292" t="n">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="H292" t="inlineStr">
         <is>
@@ -14877,7 +14877,7 @@
         <v>15588</v>
       </c>
       <c r="G295" t="n">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="H295" t="inlineStr">
         <is>
@@ -14926,7 +14926,7 @@
         <v>10915</v>
       </c>
       <c r="G296" t="n">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="H296" t="inlineStr">
         <is>
@@ -15021,7 +15021,7 @@
         </is>
       </c>
       <c r="F298" t="n">
-        <v>4573</v>
+        <v>4574</v>
       </c>
       <c r="G298" t="n">
         <v>165</v>
@@ -15073,7 +15073,7 @@
         <v>16388</v>
       </c>
       <c r="G299" t="n">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="H299" t="inlineStr">
         <is>
@@ -15119,10 +15119,10 @@
         </is>
       </c>
       <c r="F300" t="n">
-        <v>39889</v>
+        <v>39890</v>
       </c>
       <c r="G300" t="n">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="H300" t="inlineStr">
         <is>
@@ -15171,7 +15171,7 @@
         <v>14250</v>
       </c>
       <c r="G301" t="n">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="H301" t="inlineStr">
         <is>
@@ -15266,10 +15266,10 @@
         </is>
       </c>
       <c r="F303" t="n">
-        <v>27983</v>
+        <v>27984</v>
       </c>
       <c r="G303" t="n">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="H303" t="inlineStr">
         <is>
@@ -15367,7 +15367,7 @@
         <v>10653</v>
       </c>
       <c r="G305" t="n">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="H305" t="inlineStr">
         <is>
@@ -15514,7 +15514,7 @@
         <v>8912</v>
       </c>
       <c r="G308" t="n">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="H308" t="inlineStr">
         <is>
@@ -15563,7 +15563,7 @@
         <v>17493</v>
       </c>
       <c r="G309" t="n">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="H309" t="inlineStr">
         <is>
@@ -15658,10 +15658,10 @@
         </is>
       </c>
       <c r="F311" t="n">
-        <v>18679</v>
+        <v>18686</v>
       </c>
       <c r="G311" t="n">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H311" t="inlineStr">
         <is>
@@ -15707,7 +15707,7 @@
         </is>
       </c>
       <c r="F312" t="n">
-        <v>4670</v>
+        <v>4671</v>
       </c>
       <c r="G312" t="n">
         <v>170</v>
@@ -15756,10 +15756,10 @@
         </is>
       </c>
       <c r="F313" t="n">
-        <v>26638</v>
+        <v>26639</v>
       </c>
       <c r="G313" t="n">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="H313" t="inlineStr">
         <is>
@@ -15805,7 +15805,7 @@
         </is>
       </c>
       <c r="F314" t="n">
-        <v>6993</v>
+        <v>6995</v>
       </c>
       <c r="G314" t="n">
         <v>284</v>
@@ -15854,10 +15854,10 @@
         </is>
       </c>
       <c r="F315" t="n">
-        <v>14286</v>
+        <v>14289</v>
       </c>
       <c r="G315" t="n">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="H315" t="inlineStr">
         <is>
@@ -15903,10 +15903,10 @@
         </is>
       </c>
       <c r="F316" t="n">
-        <v>758565</v>
+        <v>759130</v>
       </c>
       <c r="G316" t="n">
-        <v>30676</v>
+        <v>30688</v>
       </c>
       <c r="H316" t="inlineStr">
         <is>
@@ -16004,7 +16004,7 @@
         <v>21930</v>
       </c>
       <c r="G318" t="n">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="H318" t="inlineStr">
         <is>
@@ -16053,7 +16053,7 @@
         <v>14459</v>
       </c>
       <c r="G319" t="n">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="H319" t="inlineStr">
         <is>
@@ -16148,7 +16148,7 @@
         </is>
       </c>
       <c r="F321" t="n">
-        <v>7280</v>
+        <v>7281</v>
       </c>
       <c r="G321" t="n">
         <v>187</v>
@@ -16687,7 +16687,7 @@
         </is>
       </c>
       <c r="F332" t="n">
-        <v>56863</v>
+        <v>56865</v>
       </c>
       <c r="G332" t="n">
         <v>3219</v>
@@ -17030,10 +17030,10 @@
         </is>
       </c>
       <c r="F339" t="n">
-        <v>23609</v>
+        <v>23610</v>
       </c>
       <c r="G339" t="n">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="H339" t="inlineStr">
         <is>
@@ -17569,10 +17569,10 @@
         </is>
       </c>
       <c r="F350" t="n">
-        <v>326375</v>
+        <v>326404</v>
       </c>
       <c r="G350" t="n">
-        <v>24667</v>
+        <v>24669</v>
       </c>
       <c r="H350" t="inlineStr">
         <is>
@@ -18157,7 +18157,7 @@
         </is>
       </c>
       <c r="F362" t="n">
-        <v>6696</v>
+        <v>6698</v>
       </c>
       <c r="G362" t="n">
         <v>252</v>
@@ -18255,7 +18255,7 @@
         </is>
       </c>
       <c r="F364" t="n">
-        <v>22377</v>
+        <v>22378</v>
       </c>
       <c r="G364" t="n">
         <v>1471</v>
@@ -19333,7 +19333,7 @@
         </is>
       </c>
       <c r="F386" t="n">
-        <v>32586</v>
+        <v>32594</v>
       </c>
       <c r="G386" t="n">
         <v>2170</v>
@@ -20264,7 +20264,7 @@
         </is>
       </c>
       <c r="F405" t="n">
-        <v>222283</v>
+        <v>222297</v>
       </c>
       <c r="G405" t="n">
         <v>7529</v>
@@ -20411,7 +20411,7 @@
         </is>
       </c>
       <c r="F408" t="n">
-        <v>22750</v>
+        <v>22751</v>
       </c>
       <c r="G408" t="n">
         <v>1831</v>
@@ -20754,10 +20754,10 @@
         </is>
       </c>
       <c r="F415" t="n">
-        <v>255814</v>
+        <v>255846</v>
       </c>
       <c r="G415" t="n">
-        <v>8194</v>
+        <v>8195</v>
       </c>
       <c r="H415" t="inlineStr">
         <is>
@@ -21244,7 +21244,7 @@
         </is>
       </c>
       <c r="F425" t="n">
-        <v>65563</v>
+        <v>65583</v>
       </c>
       <c r="G425" t="n">
         <v>1816</v>
@@ -21587,7 +21587,7 @@
         </is>
       </c>
       <c r="F432" t="n">
-        <v>274797</v>
+        <v>274825</v>
       </c>
       <c r="G432" t="n">
         <v>7736</v>
@@ -21734,7 +21734,7 @@
         </is>
       </c>
       <c r="F435" t="n">
-        <v>181689</v>
+        <v>181691</v>
       </c>
       <c r="G435" t="n">
         <v>4815</v>
@@ -21783,7 +21783,7 @@
         </is>
       </c>
       <c r="F436" t="n">
-        <v>25010</v>
+        <v>25011</v>
       </c>
       <c r="G436" t="n">
         <v>1774</v>
@@ -21930,7 +21930,7 @@
         </is>
       </c>
       <c r="F439" t="n">
-        <v>326751</v>
+        <v>326802</v>
       </c>
       <c r="G439" t="n">
         <v>10344</v>
@@ -22469,7 +22469,7 @@
         </is>
       </c>
       <c r="F450" t="n">
-        <v>32762</v>
+        <v>32765</v>
       </c>
       <c r="G450" t="n">
         <v>1783</v>
@@ -22665,7 +22665,7 @@
         </is>
       </c>
       <c r="F454" t="n">
-        <v>9749</v>
+        <v>9751</v>
       </c>
       <c r="G454" t="n">
         <v>676</v>
@@ -23743,7 +23743,7 @@
         </is>
       </c>
       <c r="F476" t="n">
-        <v>7831</v>
+        <v>7833</v>
       </c>
       <c r="G476" t="n">
         <v>838</v>
@@ -24919,10 +24919,10 @@
         </is>
       </c>
       <c r="F500" t="n">
-        <v>119324</v>
+        <v>119354</v>
       </c>
       <c r="G500" t="n">
-        <v>1961</v>
+        <v>1962</v>
       </c>
       <c r="H500" t="inlineStr">
         <is>
@@ -25066,7 +25066,7 @@
         </is>
       </c>
       <c r="F503" t="n">
-        <v>20728</v>
+        <v>20730</v>
       </c>
       <c r="G503" t="n">
         <v>462</v>
@@ -25605,7 +25605,7 @@
         </is>
       </c>
       <c r="F514" t="n">
-        <v>140072</v>
+        <v>140117</v>
       </c>
       <c r="G514" t="n">
         <v>2472</v>
@@ -26438,10 +26438,10 @@
         </is>
       </c>
       <c r="F531" t="n">
-        <v>334390</v>
+        <v>334452</v>
       </c>
       <c r="G531" t="n">
-        <v>5611</v>
+        <v>5613</v>
       </c>
       <c r="H531" t="inlineStr">
         <is>
@@ -27320,7 +27320,7 @@
         </is>
       </c>
       <c r="F549" t="n">
-        <v>1218159</v>
+        <v>1218163</v>
       </c>
       <c r="G549" t="n">
         <v>19569</v>
@@ -27418,7 +27418,7 @@
         </is>
       </c>
       <c r="F551" t="n">
-        <v>10779</v>
+        <v>10781</v>
       </c>
       <c r="G551" t="n">
         <v>1238</v>
@@ -27467,7 +27467,7 @@
         </is>
       </c>
       <c r="F552" t="n">
-        <v>96072</v>
+        <v>96074</v>
       </c>
       <c r="G552" t="n">
         <v>2230</v>
@@ -27859,7 +27859,7 @@
         </is>
       </c>
       <c r="F560" t="n">
-        <v>179595</v>
+        <v>179600</v>
       </c>
       <c r="G560" t="n">
         <v>2968</v>
@@ -28006,7 +28006,7 @@
         </is>
       </c>
       <c r="F563" t="n">
-        <v>86031</v>
+        <v>86033</v>
       </c>
       <c r="G563" t="n">
         <v>1749</v>
@@ -28104,7 +28104,7 @@
         </is>
       </c>
       <c r="F565" t="n">
-        <v>87769</v>
+        <v>87770</v>
       </c>
       <c r="G565" t="n">
         <v>1590</v>
@@ -28153,7 +28153,7 @@
         </is>
       </c>
       <c r="F566" t="n">
-        <v>9387</v>
+        <v>9388</v>
       </c>
       <c r="G566" t="n">
         <v>1127</v>
@@ -28545,7 +28545,7 @@
         </is>
       </c>
       <c r="F574" t="n">
-        <v>89331</v>
+        <v>89333</v>
       </c>
       <c r="G574" t="n">
         <v>1863</v>
@@ -28643,7 +28643,7 @@
         </is>
       </c>
       <c r="F576" t="n">
-        <v>77554</v>
+        <v>77555</v>
       </c>
       <c r="G576" t="n">
         <v>1495</v>
@@ -28839,7 +28839,7 @@
         </is>
       </c>
       <c r="F580" t="n">
-        <v>98344</v>
+        <v>98349</v>
       </c>
       <c r="G580" t="n">
         <v>1774</v>
@@ -28937,10 +28937,10 @@
         </is>
       </c>
       <c r="F582" t="n">
-        <v>499264</v>
+        <v>499298</v>
       </c>
       <c r="G582" t="n">
-        <v>8619</v>
+        <v>8618</v>
       </c>
       <c r="H582" t="inlineStr">
         <is>
@@ -29035,7 +29035,7 @@
         </is>
       </c>
       <c r="F584" t="n">
-        <v>43584</v>
+        <v>43585</v>
       </c>
       <c r="G584" t="n">
         <v>1065</v>
@@ -29378,7 +29378,7 @@
         </is>
       </c>
       <c r="F591" t="n">
-        <v>480566</v>
+        <v>480580</v>
       </c>
       <c r="G591" t="n">
         <v>6959</v>
@@ -29427,7 +29427,7 @@
         </is>
       </c>
       <c r="F592" t="n">
-        <v>1379888</v>
+        <v>1379929</v>
       </c>
       <c r="G592" t="n">
         <v>69805</v>
@@ -29525,7 +29525,7 @@
         </is>
       </c>
       <c r="F594" t="n">
-        <v>52110</v>
+        <v>52111</v>
       </c>
       <c r="G594" t="n">
         <v>1155</v>
@@ -29574,10 +29574,10 @@
         </is>
       </c>
       <c r="F595" t="n">
-        <v>618693</v>
+        <v>618839</v>
       </c>
       <c r="G595" t="n">
-        <v>10674</v>
+        <v>10677</v>
       </c>
       <c r="H595" t="inlineStr">
         <is>
@@ -29623,7 +29623,7 @@
         </is>
       </c>
       <c r="F596" t="n">
-        <v>158369</v>
+        <v>158370</v>
       </c>
       <c r="G596" t="n">
         <v>2634</v>
@@ -29721,7 +29721,7 @@
         </is>
       </c>
       <c r="F598" t="n">
-        <v>112879</v>
+        <v>112891</v>
       </c>
       <c r="G598" t="n">
         <v>2302</v>
@@ -29819,10 +29819,10 @@
         </is>
       </c>
       <c r="F600" t="n">
-        <v>105098</v>
+        <v>105144</v>
       </c>
       <c r="G600" t="n">
-        <v>2161</v>
+        <v>2162</v>
       </c>
       <c r="H600" t="inlineStr">
         <is>
@@ -29917,7 +29917,7 @@
         </is>
       </c>
       <c r="F602" t="n">
-        <v>251073</v>
+        <v>251078</v>
       </c>
       <c r="G602" t="n">
         <v>4452</v>
@@ -29966,7 +29966,7 @@
         </is>
       </c>
       <c r="F603" t="n">
-        <v>264397</v>
+        <v>264407</v>
       </c>
       <c r="G603" t="n">
         <v>4661</v>
@@ -30015,10 +30015,10 @@
         </is>
       </c>
       <c r="F604" t="n">
-        <v>221019</v>
+        <v>221060</v>
       </c>
       <c r="G604" t="n">
-        <v>4096</v>
+        <v>4097</v>
       </c>
       <c r="H604" t="inlineStr">
         <is>
@@ -30064,7 +30064,7 @@
         </is>
       </c>
       <c r="F605" t="n">
-        <v>515772</v>
+        <v>515803</v>
       </c>
       <c r="G605" t="n">
         <v>8960</v>
@@ -30113,10 +30113,10 @@
         </is>
       </c>
       <c r="F606" t="n">
-        <v>133659</v>
+        <v>133675</v>
       </c>
       <c r="G606" t="n">
-        <v>3855</v>
+        <v>3854</v>
       </c>
       <c r="H606" t="inlineStr">
         <is>

</xml_diff>